<commit_message>
[#664] Add sourcing principles to reducing upstream suppliers tier
</commit_message>
<xml_diff>
--- a/backend/source/transformer/procurement_library_v2_oct2025/USE-THIS _Sustainable Procurement Practices Library_Updated Changes_October 2025_1 to 5 ranking.xlsx
+++ b/backend/source/transformer/procurement_library_v2_oct2025/USE-THIS _Sustainable Procurement Practices Library_Updated Changes_October 2025_1 to 5 ranking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="236">
   <si>
     <t xml:space="preserve">Mapping to Sourcing Strategy Cycle</t>
   </si>
@@ -2427,9 +2427,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1227960</xdr:colOff>
+      <xdr:colOff>1226880</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>27720</xdr:rowOff>
+      <xdr:rowOff>26640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2439,15 +2439,15 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="133200"/>
-          <a:ext cx="1161360" cy="437400"/>
+          <a:ext cx="1160280" cy="436320"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
           <a:gdLst>
-            <a:gd name="textAreaLeft" fmla="*/ 0 w 1161360"/>
-            <a:gd name="textAreaRight" fmla="*/ 1162080 w 1161360"/>
-            <a:gd name="textAreaTop" fmla="*/ 0 h 437400"/>
-            <a:gd name="textAreaBottom" fmla="*/ 438120 h 437400"/>
+            <a:gd name="textAreaLeft" fmla="*/ 0 w 1160280"/>
+            <a:gd name="textAreaRight" fmla="*/ 1162080 w 1160280"/>
+            <a:gd name="textAreaTop" fmla="*/ 0 h 436320"/>
+            <a:gd name="textAreaBottom" fmla="*/ 438120 h 436320"/>
           </a:gdLst>
           <a:ahLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
@@ -3300,8 +3300,8 @@
   </sheetPr>
   <dimension ref="A1:AC1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3322,7 +3322,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="20.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="28.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="20.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4362,7 +4362,9 @@
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
+      <c r="I17" s="20" t="s">
+        <v>34</v>
+      </c>
       <c r="J17" s="20"/>
       <c r="K17" s="20"/>
       <c r="L17" s="20"/>
@@ -8270,7 +8272,7 @@
   <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I17 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
[#664] Incorporate income & environment into interventions step1 and 2, add sourcing principles 3 & 4 for reducing upstream tiers
</commit_message>
<xml_diff>
--- a/backend/source/transformer/procurement_library_v2_oct2025/USE-THIS _Sustainable Procurement Practices Library_Updated Changes_October 2025_1 to 5 ranking.xlsx
+++ b/backend/source/transformer/procurement_library_v2_oct2025/USE-THIS _Sustainable Procurement Practices Library_Updated Changes_October 2025_1 to 5 ranking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="237">
   <si>
     <t xml:space="preserve">Mapping to Sourcing Strategy Cycle</t>
   </si>
@@ -233,7 +233,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Income</t>
+    <t xml:space="preserve">Income, Environment</t>
   </si>
   <si>
     <t xml:space="preserve">Incorporate Business Strategy Needs </t>
@@ -290,6 +290,9 @@
     <t xml:space="preserve">Based on old procurement framework of IDH and co-developmeent with Mars
 Iterated by EY and based on interview process within the project
 Evidence of clear supplier segmentation process in Mondelez Interview with CPO LATAM, more </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Income</t>
   </si>
   <si>
     <t xml:space="preserve">Buyer Sustainability Targets</t>
@@ -1928,7 +1931,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1996,6 +1999,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="8"/>
@@ -2179,7 +2188,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2288,6 +2297,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2308,8 +2321,8 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -2324,7 +2337,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2427,9 +2444,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1226880</xdr:colOff>
+      <xdr:colOff>1226520</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>26640</xdr:rowOff>
+      <xdr:rowOff>26280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2439,15 +2456,15 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="133200"/>
-          <a:ext cx="1160280" cy="436320"/>
+          <a:ext cx="1159920" cy="435960"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
           <a:gdLst>
-            <a:gd name="textAreaLeft" fmla="*/ 0 w 1160280"/>
-            <a:gd name="textAreaRight" fmla="*/ 1162080 w 1160280"/>
-            <a:gd name="textAreaTop" fmla="*/ 0 h 436320"/>
-            <a:gd name="textAreaBottom" fmla="*/ 438120 h 436320"/>
+            <a:gd name="textAreaLeft" fmla="*/ 0 w 1159920"/>
+            <a:gd name="textAreaRight" fmla="*/ 1162080 w 1159920"/>
+            <a:gd name="textAreaTop" fmla="*/ 0 h 435960"/>
+            <a:gd name="textAreaBottom" fmla="*/ 438120 h 435960"/>
           </a:gdLst>
           <a:ahLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
@@ -3300,13 +3317,13 @@
   </sheetPr>
   <dimension ref="A1:AC1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="2" style="1" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="47.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="52.14"/>
@@ -3577,7 +3594,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="25" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
@@ -3598,22 +3615,22 @@
       <c r="N5" s="20"/>
       <c r="O5" s="20"/>
       <c r="P5" s="21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Q5" s="22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R5" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S5" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="T5" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="U5" s="23" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="V5" s="24" t="s">
         <v>50</v>
@@ -3622,7 +3639,7 @@
         <v>50</v>
       </c>
       <c r="X5" s="23" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Y5" s="6" t="n">
         <v>1</v>
@@ -3662,22 +3679,22 @@
       <c r="N6" s="20"/>
       <c r="O6" s="20"/>
       <c r="P6" s="21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Q6" s="22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="R6" s="19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S6" s="22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="T6" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="U6" s="26" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="V6" s="24" t="s">
         <v>50</v>
@@ -3686,7 +3703,7 @@
         <v>41</v>
       </c>
       <c r="X6" s="23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Y6" s="6" t="n">
         <v>5</v>
@@ -3702,8 +3719,8 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="s">
-        <v>32</v>
+      <c r="A7" s="27" t="s">
+        <v>43</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="18" t="s">
@@ -3738,22 +3755,22 @@
         <v>34</v>
       </c>
       <c r="P7" s="21" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Q7" s="22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="R7" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="S7" s="22" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="T7" s="22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="U7" s="26" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="V7" s="24" t="s">
         <v>50</v>
@@ -3762,7 +3779,7 @@
         <v>50</v>
       </c>
       <c r="X7" s="23" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Y7" s="6" t="n">
         <v>2</v>
@@ -3800,22 +3817,22 @@
       <c r="N8" s="20"/>
       <c r="O8" s="20"/>
       <c r="P8" s="21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="Q8" s="22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="R8" s="19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="S8" s="22" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="T8" s="19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="U8" s="23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="V8" s="24" t="s">
         <v>41</v>
@@ -3824,7 +3841,7 @@
         <v>41</v>
       </c>
       <c r="X8" s="23" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="Y8" s="6" t="n">
         <v>3</v>
@@ -3841,7 +3858,7 @@
     </row>
     <row r="9" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="25" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
@@ -3864,22 +3881,22 @@
       <c r="N9" s="20"/>
       <c r="O9" s="20"/>
       <c r="P9" s="21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Q9" s="22" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="R9" s="19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="S9" s="22" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="T9" s="22" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="U9" s="26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="V9" s="24" t="s">
         <v>50</v>
@@ -3888,7 +3905,7 @@
         <v>50</v>
       </c>
       <c r="X9" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Y9" s="6" t="n">
         <v>1</v>
@@ -3905,7 +3922,7 @@
     </row>
     <row r="10" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="25" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
@@ -3928,22 +3945,22 @@
       <c r="N10" s="20"/>
       <c r="O10" s="20"/>
       <c r="P10" s="21" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="Q10" s="22" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="R10" s="19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="S10" s="22" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="T10" s="22" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="U10" s="26" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="V10" s="24" t="s">
         <v>41</v>
@@ -3952,7 +3969,7 @@
         <v>41</v>
       </c>
       <c r="X10" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Y10" s="6" t="n">
         <v>3</v>
@@ -3969,7 +3986,7 @@
     </row>
     <row r="11" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="25" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
@@ -3992,22 +4009,22 @@
       <c r="N11" s="20"/>
       <c r="O11" s="20"/>
       <c r="P11" s="21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q11" s="22" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="R11" s="19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S11" s="22" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="T11" s="19" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="U11" s="26" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="V11" s="24" t="s">
         <v>41</v>
@@ -4016,7 +4033,7 @@
         <v>50</v>
       </c>
       <c r="X11" s="23" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="Y11" s="6" t="n">
         <v>5</v>
@@ -4033,7 +4050,7 @@
     </row>
     <row r="12" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="25" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -4054,22 +4071,22 @@
       <c r="N12" s="20"/>
       <c r="O12" s="20"/>
       <c r="P12" s="21" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Q12" s="22" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="R12" s="19" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="S12" s="22" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="T12" s="22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="U12" s="26" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="V12" s="24" t="s">
         <v>41</v>
@@ -4078,7 +4095,7 @@
         <v>50</v>
       </c>
       <c r="X12" s="23" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="Y12" s="6" t="n">
         <v>3</v>
@@ -4119,23 +4136,23 @@
       <c r="M13" s="20"/>
       <c r="N13" s="20"/>
       <c r="O13" s="20"/>
-      <c r="P13" s="27" t="s">
-        <v>107</v>
+      <c r="P13" s="28" t="s">
+        <v>108</v>
       </c>
       <c r="Q13" s="22" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="R13" s="19" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="S13" s="22" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="T13" s="22" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="U13" s="26" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="V13" s="24" t="s">
         <v>41</v>
@@ -4144,7 +4161,7 @@
         <v>41</v>
       </c>
       <c r="X13" s="23" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Y13" s="6" t="n">
         <v>2</v>
@@ -4161,7 +4178,7 @@
     </row>
     <row r="14" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="25" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
@@ -4182,22 +4199,22 @@
       <c r="N14" s="20"/>
       <c r="O14" s="20"/>
       <c r="P14" s="21" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Q14" s="22" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="R14" s="19" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="S14" s="22" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="T14" s="19" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="U14" s="26" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="V14" s="24" t="s">
         <v>50</v>
@@ -4206,7 +4223,7 @@
         <v>50</v>
       </c>
       <c r="X14" s="23" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="Y14" s="6" t="n">
         <v>5</v>
@@ -4246,22 +4263,22 @@
       <c r="N15" s="20"/>
       <c r="O15" s="20"/>
       <c r="P15" s="21" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="Q15" s="19" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="R15" s="19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="S15" s="22" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="T15" s="19" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="U15" s="26" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="V15" s="24" t="s">
         <v>41</v>
@@ -4270,7 +4287,7 @@
         <v>41</v>
       </c>
       <c r="X15" s="23" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Y15" s="6" t="n">
         <v>5</v>
@@ -4287,7 +4304,7 @@
     </row>
     <row r="16" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="25" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
@@ -4310,22 +4327,22 @@
       <c r="N16" s="20"/>
       <c r="O16" s="20"/>
       <c r="P16" s="21" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="Q16" s="22" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="R16" s="19" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="S16" s="22" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="T16" s="19" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="U16" s="26" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="V16" s="24" t="s">
         <v>50</v>
@@ -4334,7 +4351,7 @@
         <v>50</v>
       </c>
       <c r="X16" s="23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Y16" s="6" t="n">
         <v>2</v>
@@ -4351,7 +4368,7 @@
     </row>
     <row r="17" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="25" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
@@ -4361,7 +4378,9 @@
       <c r="E17" s="18"/>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
+      <c r="H17" s="19" t="s">
+        <v>34</v>
+      </c>
       <c r="I17" s="20" t="s">
         <v>34</v>
       </c>
@@ -4372,22 +4391,22 @@
       <c r="N17" s="20"/>
       <c r="O17" s="20"/>
       <c r="P17" s="21" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Q17" s="22" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="R17" s="19" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="S17" s="22" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="T17" s="22" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="U17" s="26" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="V17" s="24" t="s">
         <v>41</v>
@@ -4396,7 +4415,7 @@
         <v>50</v>
       </c>
       <c r="X17" s="23" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="Y17" s="6" t="n">
         <v>3</v>
@@ -4413,7 +4432,7 @@
     </row>
     <row r="18" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="25" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
@@ -4434,22 +4453,22 @@
       <c r="N18" s="20"/>
       <c r="O18" s="20"/>
       <c r="P18" s="21" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="Q18" s="22" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="R18" s="19" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="S18" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="T18" s="22" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="U18" s="26" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="V18" s="24" t="s">
         <v>41</v>
@@ -4458,7 +4477,7 @@
         <v>41</v>
       </c>
       <c r="X18" s="23" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="Y18" s="6" t="n">
         <v>3</v>
@@ -4498,22 +4517,22 @@
       <c r="N19" s="20"/>
       <c r="O19" s="20"/>
       <c r="P19" s="21" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="Q19" s="22" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="R19" s="19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="S19" s="22" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="T19" s="19" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="U19" s="26" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="V19" s="24" t="s">
         <v>41</v>
@@ -4522,7 +4541,7 @@
         <v>41</v>
       </c>
       <c r="X19" s="23" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="Y19" s="6" t="n">
         <v>3</v>
@@ -4539,7 +4558,7 @@
     </row>
     <row r="20" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="25" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
@@ -4568,22 +4587,22 @@
       <c r="N20" s="20"/>
       <c r="O20" s="20"/>
       <c r="P20" s="21" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="Q20" s="22" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="R20" s="19" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="S20" s="22" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="T20" s="19" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U20" s="26" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="V20" s="24" t="s">
         <v>50</v>
@@ -4592,7 +4611,7 @@
         <v>41</v>
       </c>
       <c r="X20" s="23" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="Y20" s="6" t="n">
         <v>3</v>
@@ -4632,22 +4651,22 @@
       <c r="N21" s="20"/>
       <c r="O21" s="20"/>
       <c r="P21" s="21" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Q21" s="19" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="R21" s="19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="S21" s="19" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="T21" s="22" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="U21" s="26" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="V21" s="24" t="s">
         <v>41</v>
@@ -4656,7 +4675,7 @@
         <v>41</v>
       </c>
       <c r="X21" s="23" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="Y21" s="6" t="n">
         <v>5</v>
@@ -4690,28 +4709,28 @@
       <c r="J22" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="29" t="s">
-        <v>170</v>
-      </c>
-      <c r="Q22" s="30" t="s">
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="R22" s="31" t="s">
+      <c r="Q22" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="S22" s="30" t="s">
+      <c r="R22" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="T22" s="31" t="s">
+      <c r="S22" s="31" t="s">
         <v>174</v>
       </c>
+      <c r="T22" s="32" t="s">
+        <v>175</v>
+      </c>
       <c r="U22" s="26" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="V22" s="24" t="s">
         <v>41</v>
@@ -4720,7 +4739,7 @@
         <v>41</v>
       </c>
       <c r="X22" s="23" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="Y22" s="6" t="n">
         <v>5</v>
@@ -4760,22 +4779,22 @@
       <c r="N23" s="20"/>
       <c r="O23" s="20"/>
       <c r="P23" s="21" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Q23" s="22" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="R23" s="19" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="S23" s="22" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="T23" s="19" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="U23" s="26" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V23" s="24" t="s">
         <v>41</v>
@@ -4784,7 +4803,7 @@
         <v>41</v>
       </c>
       <c r="X23" s="23" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="Y23" s="6" t="n">
         <v>5</v>
@@ -4801,7 +4820,7 @@
     </row>
     <row r="24" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="25" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
@@ -4828,22 +4847,22 @@
       <c r="N24" s="20"/>
       <c r="O24" s="20"/>
       <c r="P24" s="21" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="Q24" s="22" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="R24" s="19" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="S24" s="22" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="T24" s="19" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="U24" s="26" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="V24" s="24" t="s">
         <v>50</v>
@@ -4852,7 +4871,7 @@
         <v>41</v>
       </c>
       <c r="X24" s="23" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="Y24" s="6" t="n">
         <v>5</v>
@@ -4868,7 +4887,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="33" t="s">
         <v>43</v>
       </c>
       <c r="B25" s="18"/>
@@ -4890,22 +4909,22 @@
       <c r="N25" s="20"/>
       <c r="O25" s="20"/>
       <c r="P25" s="21" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="Q25" s="22" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="R25" s="19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="S25" s="22" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="T25" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="U25" s="26" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="V25" s="24" t="s">
         <v>50</v>
@@ -4930,8 +4949,8 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="17" t="s">
-        <v>32</v>
+      <c r="A26" s="27" t="s">
+        <v>43</v>
       </c>
       <c r="B26" s="18"/>
       <c r="C26" s="18" t="s">
@@ -4956,22 +4975,22 @@
       <c r="N26" s="20"/>
       <c r="O26" s="20"/>
       <c r="P26" s="21" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="Q26" s="22" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="R26" s="19" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="S26" s="22" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="T26" s="19" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U26" s="26" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="V26" s="24" t="s">
         <v>50</v>
@@ -4980,7 +4999,7 @@
         <v>50</v>
       </c>
       <c r="X26" s="23" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="Y26" s="6" t="n">
         <v>1</v>
@@ -4996,7 +5015,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="33" t="s">
         <v>43</v>
       </c>
       <c r="B27" s="18" t="s">
@@ -5032,22 +5051,22 @@
         <v>34</v>
       </c>
       <c r="P27" s="21" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="Q27" s="22" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="R27" s="19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="S27" s="22" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="T27" s="22" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="U27" s="26" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="V27" s="24" t="s">
         <v>50</v>
@@ -5073,7 +5092,7 @@
     </row>
     <row r="28" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="25" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
@@ -5094,22 +5113,22 @@
       <c r="N28" s="20"/>
       <c r="O28" s="20"/>
       <c r="P28" s="21" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="Q28" s="22" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="R28" s="19" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="S28" s="22" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="T28" s="22" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="U28" s="26" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="V28" s="24" t="s">
         <v>41</v>
@@ -5118,7 +5137,7 @@
         <v>41</v>
       </c>
       <c r="X28" s="23" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="Y28" s="6" t="n">
         <v>3</v>
@@ -5160,22 +5179,22 @@
       <c r="N29" s="20"/>
       <c r="O29" s="20"/>
       <c r="P29" s="21" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="Q29" s="22" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="R29" s="19" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="S29" s="22" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="T29" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U29" s="26" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="V29" s="24" t="s">
         <v>41</v>
@@ -5184,7 +5203,7 @@
         <v>41</v>
       </c>
       <c r="X29" s="23" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="Y29" s="6" t="n">
         <v>5</v>
@@ -5219,103 +5238,103 @@
       <c r="S30" s="26"/>
       <c r="X30" s="6"/>
       <c r="Y30" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="X31" s="6"/>
       <c r="Y31" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="X32" s="6"/>
       <c r="Y32" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="32"/>
-      <c r="M33" s="32"/>
-      <c r="N33" s="32"/>
-      <c r="O33" s="32"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="34"/>
+      <c r="L33" s="34"/>
+      <c r="M33" s="34"/>
+      <c r="N33" s="34"/>
+      <c r="O33" s="34"/>
       <c r="X33" s="6"/>
       <c r="Y33" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="X34" s="6"/>
       <c r="Y34" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="X35" s="6"/>
       <c r="Y35" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="X36" s="6"/>
       <c r="Y36" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="X37" s="6"/>
       <c r="Y37" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="X38" s="6"/>
       <c r="Y38" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="X39" s="6"/>
       <c r="Y39" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="S40" s="26"/>
       <c r="X40" s="6"/>
       <c r="Y40" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="S41" s="26"/>
       <c r="X41" s="6"/>
       <c r="Y41" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="S42" s="26"/>
       <c r="X42" s="6"/>
       <c r="Y42" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="S43" s="26"/>
       <c r="X43" s="6"/>
       <c r="Y43" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5323,77 +5342,77 @@
       <c r="S44" s="26"/>
       <c r="X44" s="6"/>
       <c r="Y44" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="S45" s="26"/>
       <c r="X45" s="6"/>
       <c r="Y45" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="S46" s="26"/>
       <c r="X46" s="6"/>
       <c r="Y46" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="S47" s="26"/>
       <c r="X47" s="6"/>
       <c r="Y47" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="S48" s="26"/>
       <c r="X48" s="6"/>
       <c r="Y48" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="S49" s="26"/>
       <c r="X49" s="6"/>
       <c r="Y49" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="S50" s="26"/>
       <c r="X50" s="6"/>
       <c r="Y50" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="S51" s="26"/>
       <c r="X51" s="6"/>
       <c r="Y51" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="S52" s="26"/>
       <c r="X52" s="6"/>
       <c r="Y52" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="S53" s="26"/>
       <c r="X53" s="6"/>
       <c r="Y53" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="S54" s="26"/>
       <c r="X54" s="6"/>
       <c r="Y54" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8271,8 +8290,8 @@
   </sheetPr>
   <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I17 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8286,70 +8305,70 @@
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="33" t="s">
-        <v>225</v>
+      <c r="A5" s="35" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="34" t="s">
-        <v>226</v>
+      <c r="A6" s="36" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="33"/>
+      <c r="A7" s="35"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="33" t="s">
-        <v>227</v>
+      <c r="A8" s="35" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="33" t="s">
-        <v>228</v>
+      <c r="A9" s="35" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="34" t="s">
-        <v>229</v>
+      <c r="A10" s="36" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="33"/>
+      <c r="A11" s="35"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="33" t="s">
-        <v>230</v>
+      <c r="A12" s="35" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="34" t="s">
-        <v>231</v>
+      <c r="A13" s="36" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="33" t="s">
-        <v>232</v>
+      <c r="A14" s="35" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="34" t="s">
-        <v>233</v>
+      <c r="A15" s="36" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="33"/>
+      <c r="A16" s="35"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="33"/>
+      <c r="A17" s="35"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="35" t="s">
-        <v>234</v>
+      <c r="A18" s="37" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="36" t="s">
-        <v>235</v>
+      <c r="A19" s="38" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>